<commit_message>
operating assumptions finished. work on working capital assumptions
</commit_message>
<xml_diff>
--- a/backend/model_year_stock.xlsx
+++ b/backend/model_year_stock.xlsx
@@ -3083,13 +3083,13 @@
         </is>
       </c>
       <c r="F79" s="144" t="n">
-        <v>200</v>
+        <v>2618</v>
       </c>
       <c r="G79" s="144" t="n">
-        <v>300</v>
+        <v>2062</v>
       </c>
       <c r="H79" s="144" t="n">
-        <v>300</v>
+        <v>1346</v>
       </c>
       <c r="I79" s="145" t="n">
         <v>300</v>

</xml_diff>